<commit_message>
publish to Heroku demo
</commit_message>
<xml_diff>
--- a/translations_for_ui.xlsx
+++ b/translations_for_ui.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="404">
   <si>
     <t>_name</t>
   </si>
@@ -1228,6 +1228,9 @@
   </si>
   <si>
     <t>exc VAT (from 250 BYN)</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:Z685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7637,9 +7640,8 @@
       <c r="C163" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="D163" s="10" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(A163,""ru"",""en"")"),"A comment")</f>
-        <v>A comment</v>
+      <c r="D163" s="20" t="s">
+        <v>403</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>

</xml_diff>